<commit_message>
cree mi primera función de excel
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariel\Downloads\CURSOS\nuevosonline\Ofimatica\Excel\practica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15F7F3D-8D34-4F23-BE36-E45C74F585A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD2E241-1A1F-47E8-A785-39A3E287170D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="0" windowWidth="20445" windowHeight="11520" activeTab="1" xr2:uid="{8B6134CC-5B2E-4F73-8CAE-13053EF6A2BA}"/>
+    <workbookView xWindow="45" yWindow="0" windowWidth="20445" windowHeight="11520" activeTab="2" xr2:uid="{8B6134CC-5B2E-4F73-8CAE-13053EF6A2BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -953,6 +953,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EE4356-0625-43C5-9481-C01F5D403C16}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AK414"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
@@ -23173,10 +23174,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1125AF-E7F3-4134-87CC-89FA5377F1C3}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24654,7 +24656,7 @@
       </c>
       <c r="P18" s="1">
         <f ca="1">TODAY()</f>
-        <v>45460</v>
+        <v>45462</v>
       </c>
       <c r="Q18">
         <v>366</v>
@@ -24970,6 +24972,9 @@
       <c r="O23" t="s">
         <v>111</v>
       </c>
+      <c r="R23">
+        <v>2</v>
+      </c>
       <c r="S23">
         <v>1</v>
       </c>
@@ -25030,6 +25035,9 @@
         <f t="array" ref="Q24">INDEX(P5:P8,Q22,1)</f>
         <v>Cerveza</v>
       </c>
+      <c r="R24">
+        <v>2</v>
+      </c>
       <c r="S24">
         <v>3</v>
       </c>
@@ -25085,6 +25093,14 @@
       </c>
       <c r="O25" t="s">
         <v>110</v>
+      </c>
+      <c r="Q25">
+        <f>SUM(S21:S26,T21:T24,_xlfn.ANCHORARRAY(U21))</f>
+        <v>31</v>
+      </c>
+      <c r="R25">
+        <f>SUM(S21:S26 R23:T24)</f>
+        <v>4</v>
       </c>
       <c r="S25">
         <v>3</v>
@@ -25712,12 +25728,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72FA39D-C6F4-4B25-AFF2-068645F310B6}">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Hoja3"/>
+  <dimension ref="B1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>6</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f>B1*C1/D1</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>